<commit_message>
excel to string[][] - dynamic records
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -386,7 +386,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,8 +411,8 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2">
+        <v>123</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
valid and invalid with excel and dataprovider
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="6180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Expected URL</t>
+  </si>
+  <si>
+    <t>Har</t>
   </si>
 </sst>
 </file>
@@ -383,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,6 +432,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -436,10 +450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,21 +484,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
created common dataprovider. make sheetname as testmethod name
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="6180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="2" r:id="rId1"/>
     <sheet name="validCredentialTest" sheetId="1" r:id="rId2"/>
+    <sheet name="addEmployeeTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -58,6 +59,15 @@
   </si>
   <si>
     <t>Har</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>wick</t>
   </si>
 </sst>
 </file>
@@ -452,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,4 +500,57 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>